<commit_message>
Este es el segundo commit del proyecto y se agrego mas
</commit_message>
<xml_diff>
--- a/prueba.xlsx
+++ b/prueba.xlsx
@@ -331,92 +331,122 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>1</v>
       </c>
       <c r="B1">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2</v>
       </c>
       <c r="B2">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>3</v>
       </c>
       <c r="B3">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>5</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
       <c r="B6">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
       <c r="B7">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
       <c r="B8">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
       <c r="B9">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>10</v>
       </c>
       <c r="B10">
         <v>5</v>
+      </c>
+      <c r="C10">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>